<commit_message>
# agregados y 17 Borrado
</commit_message>
<xml_diff>
--- a/Casos de Prueba/Match Making Results.xlsx
+++ b/Casos de Prueba/Match Making Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>A.EXE</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>#16</t>
-  </si>
-  <si>
-    <t>#17</t>
   </si>
   <si>
     <t>#10</t>
@@ -164,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -305,51 +302,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -364,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -387,17 +339,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -697,20 +645,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="18" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="23" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>10</v>
@@ -736,16 +684,16 @@
       <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="26" t="s">
         <v>18</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>19</v>
       </c>
       <c r="N1" s="15" t="s">
@@ -760,11 +708,8 @@
       <c r="Q1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -776,7 +721,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="10"/>
-      <c r="J2" s="29"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="6"/>
       <c r="L2" s="10"/>
       <c r="M2" s="6"/>
@@ -784,9 +729,8 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="18"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -798,7 +742,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="27"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
       <c r="L3" s="12"/>
       <c r="M3" s="1"/>
@@ -806,9 +750,8 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="19"/>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -820,7 +763,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="1"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="27"/>
+      <c r="J4" s="23"/>
       <c r="K4" s="2"/>
       <c r="L4" s="12"/>
       <c r="M4" s="2"/>
@@ -828,9 +771,8 @@
       <c r="O4" s="1"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="20"/>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -842,7 +784,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
       <c r="I5" s="12"/>
-      <c r="J5" s="26"/>
+      <c r="J5" s="22"/>
       <c r="K5" s="1"/>
       <c r="L5" s="12"/>
       <c r="M5" s="1"/>
@@ -850,9 +792,8 @@
       <c r="O5" s="2"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="20"/>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -864,7 +805,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="12"/>
-      <c r="J6" s="28"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="1"/>
       <c r="L6" s="12"/>
       <c r="M6" s="1"/>
@@ -872,9 +813,8 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="19"/>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -886,7 +826,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="27"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="2"/>
       <c r="L7" s="11"/>
       <c r="M7" s="2"/>
@@ -894,9 +834,8 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="19"/>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -908,7 +847,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="27"/>
+      <c r="J8" s="23"/>
       <c r="K8" s="1"/>
       <c r="L8" s="12"/>
       <c r="M8" s="1"/>
@@ -916,9 +855,8 @@
       <c r="O8" s="2"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="20"/>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -930,7 +868,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="26"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="2"/>
       <c r="L9" s="11"/>
       <c r="M9" s="2"/>
@@ -938,13 +876,12 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="20"/>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -954,8 +891,8 @@
         <v>9</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="31" t="s">
-        <v>27</v>
+      <c r="J10" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="14"/>
@@ -966,79 +903,67 @@
       </c>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="24"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q11" s="16"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q12" s="17"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="R16" s="21"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="21"/>
-    </row>
-    <row r="17" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-    </row>
-    <row r="18" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-    </row>
-    <row r="19" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-    </row>
-    <row r="20" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-    </row>
-    <row r="21" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-    </row>
-    <row r="22" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-    </row>
-    <row r="23" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R23" s="21"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
-      <c r="U23" s="21"/>
-    </row>
-    <row r="24" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R24" s="21"/>
-      <c r="S24" s="21"/>
-      <c r="T24" s="21"/>
-      <c r="U24" s="21"/>
-    </row>
-    <row r="25" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="21"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="18"/>
+    </row>
+    <row r="17" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+    </row>
+    <row r="18" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+    </row>
+    <row r="19" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+    </row>
+    <row r="20" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+    </row>
+    <row r="21" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+    </row>
+    <row r="22" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+    </row>
+    <row r="23" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+    </row>
+    <row r="24" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+    </row>
+    <row r="25" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>